<commit_message>
Add initial CIFAR-10 optimizer comparison code
Added first-code.py implementing and benchmarking several optimizers (SGD, Momentum, Adam, SR-Adam Fixed, SR-Adam Dynamic) on CIFAR-10 with a simple CNN, including data loading, training, evaluation, and result plotting. Updated .gitignore to exclude results directories. Updated main.ipynb and main.py to reflect new outputs and code structure. Minor updates to config and results files.
</commit_message>
<xml_diff>
--- a/results_CIFAR10_noise0.0/optimizer_comparison_CIFAR10_batch512_epochs20_noise0.0.xlsx
+++ b/results_CIFAR10_noise0.0/optimizer_comparison_CIFAR10_batch512_epochs20_noise0.0.xlsx
@@ -10,9 +10,9 @@
     <sheet name="SGD" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Momentum" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Adam" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="SR-Adam_Fixed,_Global" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="SR-Adam_Adaptive,_Global" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="SR-Adam_Adaptive,_Local" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="SR-Adam_Fixed_Global" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SR-Adam_Adaptive_Global" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="SR-Adam_Adaptive_Local" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -487,7 +487,7 @@
         <v>22.74</v>
       </c>
       <c r="F2" t="n">
-        <v>115.2762644290924</v>
+        <v>120.8859672546387</v>
       </c>
     </row>
     <row r="3">
@@ -507,7 +507,7 @@
         <v>27.96</v>
       </c>
       <c r="F3" t="n">
-        <v>111.9226341247559</v>
+        <v>112.536726474762</v>
       </c>
     </row>
     <row r="4">
@@ -527,7 +527,7 @@
         <v>31.59</v>
       </c>
       <c r="F4" t="n">
-        <v>112.9830708503723</v>
+        <v>111.2239947319031</v>
       </c>
     </row>
     <row r="5">
@@ -547,7 +547,7 @@
         <v>32.61</v>
       </c>
       <c r="F5" t="n">
-        <v>112.8927731513977</v>
+        <v>114.3406889438629</v>
       </c>
     </row>
     <row r="6">
@@ -567,7 +567,7 @@
         <v>34.74</v>
       </c>
       <c r="F6" t="n">
-        <v>112.3732137680054</v>
+        <v>116.9775185585022</v>
       </c>
     </row>
     <row r="7">
@@ -587,7 +587,7 @@
         <v>34.86</v>
       </c>
       <c r="F7" t="n">
-        <v>112.7131173610687</v>
+        <v>111.2345561981201</v>
       </c>
     </row>
     <row r="8">
@@ -607,7 +607,7 @@
         <v>36.33</v>
       </c>
       <c r="F8" t="n">
-        <v>112.1497328281403</v>
+        <v>119.1422913074493</v>
       </c>
     </row>
     <row r="9">
@@ -627,7 +627,7 @@
         <v>36.98</v>
       </c>
       <c r="F9" t="n">
-        <v>113.6190824508667</v>
+        <v>114.9534423351288</v>
       </c>
     </row>
     <row r="10">
@@ -647,7 +647,7 @@
         <v>39.82</v>
       </c>
       <c r="F10" t="n">
-        <v>113.194233417511</v>
+        <v>115.4654822349548</v>
       </c>
     </row>
     <row r="11">
@@ -667,7 +667,7 @@
         <v>40.55</v>
       </c>
       <c r="F11" t="n">
-        <v>112.1546123027802</v>
+        <v>113.2959833145142</v>
       </c>
     </row>
     <row r="12">
@@ -687,7 +687,7 @@
         <v>42.05</v>
       </c>
       <c r="F12" t="n">
-        <v>112.1319379806519</v>
+        <v>113.7763543128967</v>
       </c>
     </row>
     <row r="13">
@@ -707,7 +707,7 @@
         <v>42.54</v>
       </c>
       <c r="F13" t="n">
-        <v>113.4036817550659</v>
+        <v>113.0586605072021</v>
       </c>
     </row>
     <row r="14">
@@ -727,7 +727,7 @@
         <v>44.93</v>
       </c>
       <c r="F14" t="n">
-        <v>112.5665113925934</v>
+        <v>114.6656816005707</v>
       </c>
     </row>
     <row r="15">
@@ -747,7 +747,7 @@
         <v>46.83</v>
       </c>
       <c r="F15" t="n">
-        <v>112.5005192756653</v>
+        <v>113.6552605628967</v>
       </c>
     </row>
     <row r="16">
@@ -767,7 +767,7 @@
         <v>46.89</v>
       </c>
       <c r="F16" t="n">
-        <v>112.4897494316101</v>
+        <v>115.2861998081207</v>
       </c>
     </row>
     <row r="17">
@@ -787,7 +787,7 @@
         <v>46.67</v>
       </c>
       <c r="F17" t="n">
-        <v>112.9495804309845</v>
+        <v>113.2577214241028</v>
       </c>
     </row>
     <row r="18">
@@ -807,7 +807,7 @@
         <v>48.16</v>
       </c>
       <c r="F18" t="n">
-        <v>112.8533086776733</v>
+        <v>113.4298889636993</v>
       </c>
     </row>
     <row r="19">
@@ -827,7 +827,7 @@
         <v>48.58</v>
       </c>
       <c r="F19" t="n">
-        <v>112.7162888050079</v>
+        <v>113.1418569087982</v>
       </c>
     </row>
     <row r="20">
@@ -847,7 +847,7 @@
         <v>47.53</v>
       </c>
       <c r="F20" t="n">
-        <v>113.1974813938141</v>
+        <v>114.8227710723877</v>
       </c>
     </row>
     <row r="21">
@@ -867,7 +867,7 @@
         <v>49.33</v>
       </c>
       <c r="F21" t="n">
-        <v>113.0667676925659</v>
+        <v>114.4767460823059</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +938,7 @@
         <v>36.05</v>
       </c>
       <c r="F2" t="n">
-        <v>113.3272702693939</v>
+        <v>115.3561823368073</v>
       </c>
     </row>
     <row r="3">
@@ -958,7 +958,7 @@
         <v>45.55</v>
       </c>
       <c r="F3" t="n">
-        <v>113.1615653038025</v>
+        <v>113.4463765621185</v>
       </c>
     </row>
     <row r="4">
@@ -978,7 +978,7 @@
         <v>47.7</v>
       </c>
       <c r="F4" t="n">
-        <v>112.2793507575989</v>
+        <v>113.1467127799988</v>
       </c>
     </row>
     <row r="5">
@@ -998,7 +998,7 @@
         <v>52.71</v>
       </c>
       <c r="F5" t="n">
-        <v>112.5190200805664</v>
+        <v>112.9463150501251</v>
       </c>
     </row>
     <row r="6">
@@ -1018,7 +1018,7 @@
         <v>55.71</v>
       </c>
       <c r="F6" t="n">
-        <v>116.2006983757019</v>
+        <v>112.4712224006653</v>
       </c>
     </row>
     <row r="7">
@@ -1038,7 +1038,7 @@
         <v>59.29</v>
       </c>
       <c r="F7" t="n">
-        <v>113.3155071735382</v>
+        <v>115.0343196392059</v>
       </c>
     </row>
     <row r="8">
@@ -1058,7 +1058,7 @@
         <v>61</v>
       </c>
       <c r="F8" t="n">
-        <v>113.9422948360443</v>
+        <v>113.0829112529755</v>
       </c>
     </row>
     <row r="9">
@@ -1078,7 +1078,7 @@
         <v>62.21</v>
       </c>
       <c r="F9" t="n">
-        <v>113.5622293949127</v>
+        <v>113.2054913043976</v>
       </c>
     </row>
     <row r="10">
@@ -1098,7 +1098,7 @@
         <v>64.48</v>
       </c>
       <c r="F10" t="n">
-        <v>113.2275812625885</v>
+        <v>114.940623998642</v>
       </c>
     </row>
     <row r="11">
@@ -1118,7 +1118,7 @@
         <v>65.23</v>
       </c>
       <c r="F11" t="n">
-        <v>112.7153768539429</v>
+        <v>112.7669770717621</v>
       </c>
     </row>
     <row r="12">
@@ -1138,7 +1138,7 @@
         <v>65.95999999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>113.8871409893036</v>
+        <v>111.7202303409576</v>
       </c>
     </row>
     <row r="13">
@@ -1158,7 +1158,7 @@
         <v>66.27</v>
       </c>
       <c r="F13" t="n">
-        <v>114.6979637145996</v>
+        <v>116.6967432498932</v>
       </c>
     </row>
     <row r="14">
@@ -1178,7 +1178,7 @@
         <v>67.05</v>
       </c>
       <c r="F14" t="n">
-        <v>115.534083366394</v>
+        <v>115.2928586006165</v>
       </c>
     </row>
     <row r="15">
@@ -1198,7 +1198,7 @@
         <v>68.73</v>
       </c>
       <c r="F15" t="n">
-        <v>114.368346452713</v>
+        <v>113.3775980472565</v>
       </c>
     </row>
     <row r="16">
@@ -1218,7 +1218,7 @@
         <v>69.29000000000001</v>
       </c>
       <c r="F16" t="n">
-        <v>114.0051307678223</v>
+        <v>115.2374029159546</v>
       </c>
     </row>
     <row r="17">
@@ -1238,7 +1238,7 @@
         <v>70.09</v>
       </c>
       <c r="F17" t="n">
-        <v>115.2481362819672</v>
+        <v>114.125198841095</v>
       </c>
     </row>
     <row r="18">
@@ -1258,7 +1258,7 @@
         <v>70.78</v>
       </c>
       <c r="F18" t="n">
-        <v>114.0179948806763</v>
+        <v>111.6325993537903</v>
       </c>
     </row>
     <row r="19">
@@ -1278,7 +1278,7 @@
         <v>70.59999999999999</v>
       </c>
       <c r="F19" t="n">
-        <v>112.6841535568237</v>
+        <v>115.248722076416</v>
       </c>
     </row>
     <row r="20">
@@ -1298,7 +1298,7 @@
         <v>71.08</v>
       </c>
       <c r="F20" t="n">
-        <v>112.299120426178</v>
+        <v>113.3847122192383</v>
       </c>
     </row>
     <row r="21">
@@ -1318,7 +1318,7 @@
         <v>72.38</v>
       </c>
       <c r="F21" t="n">
-        <v>114.5138425827026</v>
+        <v>116.1666924953461</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1389,7 @@
         <v>46.55</v>
       </c>
       <c r="F2" t="n">
-        <v>113.9483776092529</v>
+        <v>125.3221569061279</v>
       </c>
     </row>
     <row r="3">
@@ -1409,7 +1409,7 @@
         <v>55.84</v>
       </c>
       <c r="F3" t="n">
-        <v>112.7431163787842</v>
+        <v>118.8940362930298</v>
       </c>
     </row>
     <row r="4">
@@ -1429,7 +1429,7 @@
         <v>58.55</v>
       </c>
       <c r="F4" t="n">
-        <v>112.5238127708435</v>
+        <v>118.4653053283691</v>
       </c>
     </row>
     <row r="5">
@@ -1449,7 +1449,7 @@
         <v>63.37</v>
       </c>
       <c r="F5" t="n">
-        <v>112.7582716941833</v>
+        <v>116.5388135910034</v>
       </c>
     </row>
     <row r="6">
@@ -1469,7 +1469,7 @@
         <v>64.77</v>
       </c>
       <c r="F6" t="n">
-        <v>112.3210985660553</v>
+        <v>115.6926271915436</v>
       </c>
     </row>
     <row r="7">
@@ -1489,7 +1489,7 @@
         <v>65.59999999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>115.4154770374298</v>
+        <v>115.4822013378143</v>
       </c>
     </row>
     <row r="8">
@@ -1509,7 +1509,7 @@
         <v>67.95</v>
       </c>
       <c r="F8" t="n">
-        <v>116.2982573509216</v>
+        <v>120.677990436554</v>
       </c>
     </row>
     <row r="9">
@@ -1529,7 +1529,7 @@
         <v>68.59</v>
       </c>
       <c r="F9" t="n">
-        <v>113.7203741073608</v>
+        <v>115.5687580108643</v>
       </c>
     </row>
     <row r="10">
@@ -1549,7 +1549,7 @@
         <v>69.03</v>
       </c>
       <c r="F10" t="n">
-        <v>113.9463233947754</v>
+        <v>117.342707157135</v>
       </c>
     </row>
     <row r="11">
@@ -1569,7 +1569,7 @@
         <v>70.48</v>
       </c>
       <c r="F11" t="n">
-        <v>113.2392301559448</v>
+        <v>118.2873983383179</v>
       </c>
     </row>
     <row r="12">
@@ -1589,7 +1589,7 @@
         <v>69.22</v>
       </c>
       <c r="F12" t="n">
-        <v>122.6474938392639</v>
+        <v>118.7454588413239</v>
       </c>
     </row>
     <row r="13">
@@ -1609,7 +1609,7 @@
         <v>71.17</v>
       </c>
       <c r="F13" t="n">
-        <v>122.5075063705444</v>
+        <v>119.9983556270599</v>
       </c>
     </row>
     <row r="14">
@@ -1629,7 +1629,7 @@
         <v>72.64</v>
       </c>
       <c r="F14" t="n">
-        <v>124.9419865608215</v>
+        <v>126.6055901050568</v>
       </c>
     </row>
     <row r="15">
@@ -1649,7 +1649,7 @@
         <v>72.94</v>
       </c>
       <c r="F15" t="n">
-        <v>126.4220011234283</v>
+        <v>126.7695987224579</v>
       </c>
     </row>
     <row r="16">
@@ -1669,7 +1669,7 @@
         <v>72.63</v>
       </c>
       <c r="F16" t="n">
-        <v>126.0281579494476</v>
+        <v>120.130530834198</v>
       </c>
     </row>
     <row r="17">
@@ -1689,7 +1689,7 @@
         <v>73.48</v>
       </c>
       <c r="F17" t="n">
-        <v>123.2607471942902</v>
+        <v>118.6035389900208</v>
       </c>
     </row>
     <row r="18">
@@ -1709,7 +1709,7 @@
         <v>72.98</v>
       </c>
       <c r="F18" t="n">
-        <v>116.3534302711487</v>
+        <v>120.9128932952881</v>
       </c>
     </row>
     <row r="19">
@@ -1729,7 +1729,7 @@
         <v>74.19</v>
       </c>
       <c r="F19" t="n">
-        <v>116.9599847793579</v>
+        <v>120.0609896183014</v>
       </c>
     </row>
     <row r="20">
@@ -1749,7 +1749,7 @@
         <v>73.97</v>
       </c>
       <c r="F20" t="n">
-        <v>117.1223657131195</v>
+        <v>120.6183745861053</v>
       </c>
     </row>
     <row r="21">
@@ -1769,7 +1769,7 @@
         <v>75.48</v>
       </c>
       <c r="F21" t="n">
-        <v>116.1310353279114</v>
+        <v>118.4122352600098</v>
       </c>
     </row>
   </sheetData>
@@ -1840,7 +1840,7 @@
         <v>49.62</v>
       </c>
       <c r="F2" t="n">
-        <v>116.7557651996613</v>
+        <v>127.49165391922</v>
       </c>
     </row>
     <row r="3">
@@ -1860,7 +1860,7 @@
         <v>57.21</v>
       </c>
       <c r="F3" t="n">
-        <v>115.8827948570251</v>
+        <v>119.3145108222961</v>
       </c>
     </row>
     <row r="4">
@@ -1880,7 +1880,7 @@
         <v>60.13</v>
       </c>
       <c r="F4" t="n">
-        <v>116.1080114841461</v>
+        <v>117.8959360122681</v>
       </c>
     </row>
     <row r="5">
@@ -1900,7 +1900,7 @@
         <v>64</v>
       </c>
       <c r="F5" t="n">
-        <v>115.9559600353241</v>
+        <v>124.1882529258728</v>
       </c>
     </row>
     <row r="6">
@@ -1920,7 +1920,7 @@
         <v>64.01000000000001</v>
       </c>
       <c r="F6" t="n">
-        <v>116.6518187522888</v>
+        <v>116.3647351264954</v>
       </c>
     </row>
     <row r="7">
@@ -1940,7 +1940,7 @@
         <v>66.89</v>
       </c>
       <c r="F7" t="n">
-        <v>115.7581012248993</v>
+        <v>115.3504228591919</v>
       </c>
     </row>
     <row r="8">
@@ -1960,7 +1960,7 @@
         <v>69.03</v>
       </c>
       <c r="F8" t="n">
-        <v>114.6869235038757</v>
+        <v>119.0081334114075</v>
       </c>
     </row>
     <row r="9">
@@ -1980,7 +1980,7 @@
         <v>69.84</v>
       </c>
       <c r="F9" t="n">
-        <v>115.4704837799072</v>
+        <v>115.0275444984436</v>
       </c>
     </row>
     <row r="10">
@@ -2000,7 +2000,7 @@
         <v>70</v>
       </c>
       <c r="F10" t="n">
-        <v>116.5301916599274</v>
+        <v>112.0073421001434</v>
       </c>
     </row>
     <row r="11">
@@ -2020,7 +2020,7 @@
         <v>70.39</v>
       </c>
       <c r="F11" t="n">
-        <v>116.2961366176605</v>
+        <v>105.8630814552307</v>
       </c>
     </row>
     <row r="12">
@@ -2040,7 +2040,7 @@
         <v>72.05</v>
       </c>
       <c r="F12" t="n">
-        <v>115.514997959137</v>
+        <v>104.9339964389801</v>
       </c>
     </row>
     <row r="13">
@@ -2060,7 +2060,7 @@
         <v>72.59</v>
       </c>
       <c r="F13" t="n">
-        <v>115.3492774963379</v>
+        <v>108.3566949367523</v>
       </c>
     </row>
     <row r="14">
@@ -2080,7 +2080,7 @@
         <v>72.37</v>
       </c>
       <c r="F14" t="n">
-        <v>115.0199468135834</v>
+        <v>109.4579603672028</v>
       </c>
     </row>
     <row r="15">
@@ -2100,7 +2100,7 @@
         <v>72.95</v>
       </c>
       <c r="F15" t="n">
-        <v>116.0468664169312</v>
+        <v>112.0998058319092</v>
       </c>
     </row>
     <row r="16">
@@ -2120,7 +2120,7 @@
         <v>73.38</v>
       </c>
       <c r="F16" t="n">
-        <v>116.272488117218</v>
+        <v>108.070769071579</v>
       </c>
     </row>
     <row r="17">
@@ -2140,7 +2140,7 @@
         <v>73.83</v>
       </c>
       <c r="F17" t="n">
-        <v>116.8740639686584</v>
+        <v>107.1583218574524</v>
       </c>
     </row>
     <row r="18">
@@ -2160,7 +2160,7 @@
         <v>74.56999999999999</v>
       </c>
       <c r="F18" t="n">
-        <v>118.6990902423859</v>
+        <v>104.9762935638428</v>
       </c>
     </row>
     <row r="19">
@@ -2180,7 +2180,7 @@
         <v>74.5</v>
       </c>
       <c r="F19" t="n">
-        <v>117.2316961288452</v>
+        <v>104.7354953289032</v>
       </c>
     </row>
     <row r="20">
@@ -2200,7 +2200,7 @@
         <v>75.23999999999999</v>
       </c>
       <c r="F20" t="n">
-        <v>115.4388628005981</v>
+        <v>105.4344363212585</v>
       </c>
     </row>
     <row r="21">
@@ -2220,7 +2220,7 @@
         <v>75.31999999999999</v>
       </c>
       <c r="F21" t="n">
-        <v>116.1188044548035</v>
+        <v>108.2003445625305</v>
       </c>
     </row>
   </sheetData>
@@ -2279,19 +2279,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>29.7042108020004</v>
+        <v>1.770654905815514</v>
       </c>
       <c r="C2" t="n">
-        <v>34.21297159194946</v>
+        <v>1.440768057107925</v>
       </c>
       <c r="D2" t="n">
-        <v>10.986</v>
+        <v>35.21</v>
       </c>
       <c r="E2" t="n">
-        <v>11.64</v>
+        <v>48.11</v>
       </c>
       <c r="F2" t="n">
-        <v>114.5728535652161</v>
+        <v>115.2215192317963</v>
       </c>
     </row>
     <row r="3">
@@ -2299,19 +2299,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>79.12262951597876</v>
+        <v>1.462679386138916</v>
       </c>
       <c r="C3" t="n">
-        <v>20.99938707351685</v>
+        <v>1.264407747983932</v>
       </c>
       <c r="D3" t="n">
-        <v>10.954</v>
+        <v>47.16</v>
       </c>
       <c r="E3" t="n">
-        <v>10.67</v>
+        <v>54.84</v>
       </c>
       <c r="F3" t="n">
-        <v>115.5065155029297</v>
+        <v>113.0916621685028</v>
       </c>
     </row>
     <row r="4">
@@ -2319,19 +2319,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>5.371912321265863</v>
+        <v>1.335375037728524</v>
       </c>
       <c r="C4" t="n">
-        <v>2.371704471111298</v>
+        <v>1.134999012947083</v>
       </c>
       <c r="D4" t="n">
-        <v>10.088</v>
+        <v>51.786</v>
       </c>
       <c r="E4" t="n">
-        <v>10.07</v>
+        <v>60.14</v>
       </c>
       <c r="F4" t="n">
-        <v>115.2065093517303</v>
+        <v>117.1261639595032</v>
       </c>
     </row>
     <row r="5">
@@ -2339,19 +2339,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2.348076878761759</v>
+        <v>1.229177420236626</v>
       </c>
       <c r="C5" t="n">
-        <v>2.349870991706848</v>
+        <v>1.05806211233139</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>55.998</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>62.26</v>
       </c>
       <c r="F5" t="n">
-        <v>116.5995280742645</v>
+        <v>115.4685640335083</v>
       </c>
     </row>
     <row r="6">
@@ -2359,19 +2359,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2.424887910181162</v>
+        <v>1.17272836943062</v>
       </c>
       <c r="C6" t="n">
-        <v>2.370737767219544</v>
+        <v>0.9921803832054138</v>
       </c>
       <c r="D6" t="n">
-        <v>10.004</v>
+        <v>58.118</v>
       </c>
       <c r="E6" t="n">
-        <v>10.01</v>
+        <v>65.22</v>
       </c>
       <c r="F6" t="n">
-        <v>117.1753468513489</v>
+        <v>117.2261848449707</v>
       </c>
     </row>
     <row r="7">
@@ -2379,19 +2379,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.495196361931003</v>
+        <v>1.107803512592705</v>
       </c>
       <c r="C7" t="n">
-        <v>2.449873971939087</v>
+        <v>0.9533442407846451</v>
       </c>
       <c r="D7" t="n">
-        <v>10.01</v>
+        <v>60.56</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>66.42</v>
       </c>
       <c r="F7" t="n">
-        <v>116.5027089118958</v>
+        <v>115.2095839977264</v>
       </c>
     </row>
     <row r="8">
@@ -2399,227 +2399,279 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>2.482927833284651</v>
+        <v>1.071534172004583</v>
       </c>
       <c r="C8" t="n">
-        <v>2.538194930553436</v>
+        <v>0.9081777989864349</v>
       </c>
       <c r="D8" t="n">
-        <v>10.008</v>
+        <v>61.872</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>67.91</v>
       </c>
       <c r="F8" t="n">
-        <v>116.9680151939392</v>
+        <v>116.2051680088043</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>1.04722928575107</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.909335058927536</v>
+      </c>
       <c r="D9" t="n">
-        <v>10.004</v>
+        <v>62.786</v>
       </c>
       <c r="E9" t="n">
-        <v>10.01</v>
+        <v>67.98</v>
       </c>
       <c r="F9" t="n">
-        <v>116.2876350879669</v>
+        <v>115.7117159366608</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>1.012026738147346</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.9032434403896332</v>
+      </c>
       <c r="D10" t="n">
-        <v>10.034</v>
+        <v>64.244</v>
       </c>
       <c r="E10" t="n">
-        <v>10.02</v>
+        <v>68.84999999999999</v>
       </c>
       <c r="F10" t="n">
-        <v>116.3432142734528</v>
+        <v>117.2253956794739</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>0.9935218764811146</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8499372333288193</v>
+      </c>
       <c r="D11" t="n">
-        <v>10.028</v>
+        <v>64.648</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>70.26000000000001</v>
       </c>
       <c r="F11" t="n">
-        <v>116.4278934001923</v>
+        <v>117.6430552005768</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>0.9747475647196477</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.8393780320882798</v>
+      </c>
       <c r="D12" t="n">
-        <v>10</v>
+        <v>65.58</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>71.48999999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>115.836275100708</v>
+        <v>120.719263792038</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>0.9580985952396782</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.838104572892189</v>
+      </c>
       <c r="D13" t="n">
-        <v>10</v>
+        <v>66.282</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>70.48</v>
       </c>
       <c r="F13" t="n">
-        <v>117.1701509952545</v>
+        <v>120.4784531593323</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
+      <c r="B14" t="n">
+        <v>0.9305694754026375</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8005858868360519</v>
+      </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>67.158</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>72.34</v>
       </c>
       <c r="F14" t="n">
-        <v>115.7642705440521</v>
+        <v>117.5445692539215</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>0.9207288726251952</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.7877828419208527</v>
+      </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>67.408</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>72.38</v>
       </c>
       <c r="F15" t="n">
-        <v>115.6966278553009</v>
+        <v>113.8424599170685</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>0.907168090951686</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8083312451839447</v>
+      </c>
       <c r="D16" t="n">
-        <v>10</v>
+        <v>67.916</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>71.66</v>
       </c>
       <c r="F16" t="n">
-        <v>115.5860741138458</v>
+        <v>117.0502634048462</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+      <c r="B17" t="n">
+        <v>0.8964594724226971</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.7821955382823944</v>
+      </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>68.20399999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>72.48999999999999</v>
       </c>
       <c r="F17" t="n">
-        <v>119.2181303501129</v>
+        <v>117.2551326751709</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
+      <c r="B18" t="n">
+        <v>0.8810505179726348</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.7655546963214874</v>
+      </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>68.904</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F18" t="n">
-        <v>121.2923243045807</v>
+        <v>114.5344135761261</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
+      <c r="B19" t="n">
+        <v>0.8635755984150634</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.7521736085414886</v>
+      </c>
       <c r="D19" t="n">
-        <v>10</v>
+        <v>69.54000000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>73.98999999999999</v>
       </c>
       <c r="F19" t="n">
-        <v>122.2213664054871</v>
+        <v>113.2143371105194</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="B20" t="n">
+        <v>0.8505377866783921</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.7443405210971832</v>
+      </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>69.736</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>74.47</v>
       </c>
       <c r="F20" t="n">
-        <v>120.8954951763153</v>
+        <v>114.3607976436615</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+      <c r="B21" t="n">
+        <v>0.8441192446922769</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.7292491346597672</v>
+      </c>
       <c r="D21" t="n">
-        <v>10</v>
+        <v>70.3</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="F21" t="n">
-        <v>124.6696405410767</v>
+        <v>116.4618103504181</v>
       </c>
     </row>
   </sheetData>
@@ -2678,19 +2730,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>39.6808847213278</v>
+        <v>1.787590271356154</v>
       </c>
       <c r="C2" t="n">
-        <v>29.42023315429687</v>
+        <v>1.446015506982803</v>
       </c>
       <c r="D2" t="n">
-        <v>11.266</v>
+        <v>34.756</v>
       </c>
       <c r="E2" t="n">
-        <v>20.66</v>
+        <v>47.55</v>
       </c>
       <c r="F2" t="n">
-        <v>123.1566224098206</v>
+        <v>116.3999135494232</v>
       </c>
     </row>
     <row r="3">
@@ -2698,19 +2750,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>59.5304545261422</v>
+        <v>1.468139086450849</v>
       </c>
       <c r="C3" t="n">
-        <v>3.062560510635376</v>
+        <v>1.271992182731629</v>
       </c>
       <c r="D3" t="n">
-        <v>13.196</v>
+        <v>46.916</v>
       </c>
       <c r="E3" t="n">
-        <v>11.3</v>
+        <v>54.6</v>
       </c>
       <c r="F3" t="n">
-        <v>122.3674130439758</v>
+        <v>116.9149041175842</v>
       </c>
     </row>
     <row r="4">
@@ -2718,19 +2770,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2.427025128384026</v>
+        <v>1.333203674579153</v>
       </c>
       <c r="C4" t="n">
-        <v>2.517526090145111</v>
+        <v>1.153675699234009</v>
       </c>
       <c r="D4" t="n">
-        <v>10.206</v>
+        <v>52.076</v>
       </c>
       <c r="E4" t="n">
-        <v>9.99</v>
+        <v>58.76</v>
       </c>
       <c r="F4" t="n">
-        <v>120.9172208309174</v>
+        <v>123.2720973491669</v>
       </c>
     </row>
     <row r="5">
@@ -2738,19 +2790,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2.399599673796673</v>
+        <v>1.236082342206215</v>
       </c>
       <c r="C5" t="n">
-        <v>2.916831362247467</v>
+        <v>1.05967258810997</v>
       </c>
       <c r="D5" t="n">
-        <v>9.978</v>
+        <v>55.562</v>
       </c>
       <c r="E5" t="n">
-        <v>9.869999999999999</v>
+        <v>61.96</v>
       </c>
       <c r="F5" t="n">
-        <v>123.2211782932281</v>
+        <v>138.1697862148285</v>
       </c>
     </row>
     <row r="6">
@@ -2758,19 +2810,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2.558179157120841</v>
+        <v>1.17216591324125</v>
       </c>
       <c r="C6" t="n">
-        <v>3.162668204307556</v>
+        <v>1.008965846896172</v>
       </c>
       <c r="D6" t="n">
-        <v>9.988</v>
+        <v>58.162</v>
       </c>
       <c r="E6" t="n">
-        <v>9.94</v>
+        <v>63.88</v>
       </c>
       <c r="F6" t="n">
-        <v>121.4237825870514</v>
+        <v>135.2307939529419</v>
       </c>
     </row>
     <row r="7">
@@ -2778,19 +2830,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.555708009369519</v>
+        <v>1.122348476429375</v>
       </c>
       <c r="C7" t="n">
-        <v>3.684760200977325</v>
+        <v>0.9714230805635452</v>
       </c>
       <c r="D7" t="n">
-        <v>9.986000000000001</v>
+        <v>59.968</v>
       </c>
       <c r="E7" t="n">
-        <v>9.98</v>
+        <v>66.20999999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>120.8747489452362</v>
+        <v>130.8240079879761</v>
       </c>
     </row>
     <row r="8">
@@ -2798,229 +2850,279 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>2.578441641768631</v>
+        <v>1.080432648561439</v>
       </c>
       <c r="C8" t="n">
-        <v>3.920019721984863</v>
+        <v>0.9308628171682358</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>61.596</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>67.81999999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>114.7067878246307</v>
+        <v>119.1664199829102</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>1.05122249223748</v>
+      </c>
       <c r="C9" t="n">
-        <v>5.36717963218689</v>
+        <v>0.9156822770833969</v>
       </c>
       <c r="D9" t="n">
-        <v>9.997999999999999</v>
+        <v>62.896</v>
       </c>
       <c r="E9" t="n">
-        <v>9.99</v>
+        <v>68.28</v>
       </c>
       <c r="F9" t="n">
-        <v>113.2546088695526</v>
+        <v>120.8401031494141</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>1.019835274438469</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.9041554808616639</v>
+      </c>
       <c r="D10" t="n">
-        <v>9.997999999999999</v>
+        <v>63.92</v>
       </c>
       <c r="E10" t="n">
-        <v>10.03</v>
+        <v>67.88</v>
       </c>
       <c r="F10" t="n">
-        <v>112.4829766750336</v>
+        <v>120.4717638492584</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>0.989623447462004</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8700560003519058</v>
+      </c>
       <c r="D11" t="n">
-        <v>10.008</v>
+        <v>64.886</v>
       </c>
       <c r="E11" t="n">
-        <v>10.1</v>
+        <v>69.63</v>
       </c>
       <c r="F11" t="n">
-        <v>111.9919321537018</v>
+        <v>122.189001083374</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>0.9742210574296056</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.8460936546325684</v>
+      </c>
       <c r="D12" t="n">
-        <v>10.054</v>
+        <v>65.76600000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>10.25</v>
+        <v>70.2</v>
       </c>
       <c r="F12" t="n">
-        <v>113.6256666183472</v>
+        <v>117.2734642028809</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>0.9524868690237707</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8263706207275391</v>
+      </c>
       <c r="D13" t="n">
-        <v>10.15</v>
+        <v>66.182</v>
       </c>
       <c r="E13" t="n">
-        <v>10.35</v>
+        <v>71.27</v>
       </c>
       <c r="F13" t="n">
-        <v>114.3465049266815</v>
+        <v>112.8765242099762</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
+      <c r="B14" t="n">
+        <v>0.9419166561292143</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8393696457147598</v>
+      </c>
       <c r="D14" t="n">
-        <v>9.996</v>
+        <v>66.88</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>70.83</v>
       </c>
       <c r="F14" t="n">
-        <v>114.8754997253418</v>
+        <v>112.3272159099579</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>0.9223116198364569</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.7906384915113449</v>
+      </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>72.31</v>
       </c>
       <c r="F15" t="n">
-        <v>122.281530380249</v>
+        <v>111.5106000900269</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>0.9106840010808439</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8019485324621201</v>
+      </c>
       <c r="D16" t="n">
-        <v>10</v>
+        <v>67.956</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>71.69</v>
       </c>
       <c r="F16" t="n">
-        <v>119.1388690471649</v>
+        <v>111.446005821228</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+      <c r="B17" t="n">
+        <v>0.893991294564033</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.7861225187778473</v>
+      </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>68.51000000000001</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>72.84</v>
       </c>
       <c r="F17" t="n">
-        <v>118.1844472885132</v>
+        <v>112.6071808338165</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
+      <c r="B18" t="n">
+        <v>0.8830127594422321</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.7717174321413041</v>
+      </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>68.934</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>72.97</v>
       </c>
       <c r="F18" t="n">
-        <v>120.352902173996</v>
+        <v>117.0254998207092</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
+      <c r="B19" t="n">
+        <v>0.8706086855761859</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.7736718088388443</v>
+      </c>
       <c r="D19" t="n">
-        <v>10</v>
+        <v>69.34</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>73.45999999999999</v>
       </c>
       <c r="F19" t="n">
-        <v>120.1143238544464</v>
+        <v>118.5361981391907</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="B20" t="n">
+        <v>0.8605377601117504</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.7507361322641373</v>
+      </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>69.91</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>74.12</v>
       </c>
       <c r="F20" t="n">
-        <v>122.0974497795105</v>
+        <v>114.6052982807159</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+      <c r="B21" t="n">
+        <v>0.8461574644458537</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.7443847417831421</v>
+      </c>
       <c r="D21" t="n">
-        <v>10</v>
+        <v>70.434</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>74.05</v>
       </c>
       <c r="F21" t="n">
-        <v>122.1852133274078</v>
+        <v>113.9347817897797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>